<commit_message>
More Scaffolding for Effects
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet.xlsx
+++ b/IodemBot/IodemClassSheet.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4BB55B0-3095-4523-894E-948E423AA54D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D46BF0-F570-49D7-BBA2-2D5EE94DC926}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16068" windowHeight="5676" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView xWindow="0" yWindow="612" windowWidth="15360" windowHeight="9816" activeTab="2" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="135">
   <si>
     <t>Guard</t>
   </si>
@@ -372,6 +372,72 @@
   </si>
   <si>
     <t>Rockfall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cool</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Stat</t>
+  </si>
+  <si>
+    <t>Boost</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Chance</t>
+  </si>
+  <si>
+    <t>Drain</t>
+  </si>
+  <si>
+    <t>Instant Death</t>
+  </si>
+  <si>
+    <t>Reduce HP to 1</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>Vanish into Air</t>
+  </si>
+  <si>
+    <t>Double Turn</t>
+  </si>
+  <si>
+    <t>End Turn</t>
+  </si>
+  <si>
+    <t>"Lose 12% of health and may lose next turn"</t>
+  </si>
+  <si>
+    <t>May multiply damage</t>
+  </si>
+  <si>
+    <t>User Dies</t>
+  </si>
+  <si>
+    <t>Remove Condition</t>
+  </si>
+  <si>
+    <t>Param1 (string)</t>
+  </si>
+  <si>
+    <t>Param2 (int)</t>
+  </si>
+  <si>
+    <t>May ignore Defense</t>
   </si>
 </sst>
 </file>
@@ -404,12 +470,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -424,10 +508,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2B1135-77C9-499B-B6C9-9E2B30F8D34D}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,34 +854,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -894,7 +984,7 @@
         <v>26</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="M4" t="s">
         <v>26</v>
@@ -913,6 +1003,9 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
@@ -926,7 +1019,7 @@
         <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="M5" t="s">
         <v>83</v>
@@ -955,7 +1048,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B8" t="s">
@@ -967,13 +1060,13 @@
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>109</v>
       </c>
       <c r="H8" t="s">
         <v>35</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="K8" t="s">
@@ -1207,7 +1300,7 @@
         <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1258,7 +1351,7 @@
         <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
@@ -1281,7 +1374,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1317,4 +1410,134 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21AE0FE-0550-4A50-A428-F4972BDBD2F3}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ever so many more new Effects
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet.xlsx
+++ b/IodemBot/IodemClassSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5A9389-20E7-4E2E-8050-446011D0A9AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52CAE54-589C-4BAB-8AE1-D76CE3F81308}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34380" yWindow="-810" windowWidth="11850" windowHeight="9195" activeTab="2" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="135">
   <si>
     <t>Guard</t>
   </si>
@@ -438,9 +438,6 @@
   </si>
   <si>
     <t>May ignore Defense</t>
-  </si>
-  <si>
-    <t>bool</t>
   </si>
 </sst>
 </file>
@@ -1420,19 +1417,19 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B1" t="s">
@@ -1443,12 +1440,12 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
@@ -1456,7 +1453,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B4" t="s">
@@ -1465,15 +1462,12 @@
       <c r="C4" t="s">
         <v>118</v>
       </c>
-      <c r="D4" t="s">
-        <v>135</v>
-      </c>
       <c r="E4" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B5" t="s">
@@ -1501,12 +1495,12 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C8" t="s">
@@ -1522,7 +1516,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>130</v>
       </c>
       <c r="E10" t="s">

</xml_diff>

<commit_message>
new enemies line up
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet.xlsx
+++ b/IodemBot/IodemClassSheet.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4BB55B0-3095-4523-894E-948E423AA54D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52CAE54-589C-4BAB-8AE1-D76CE3F81308}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16068" windowHeight="5676" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView xWindow="34380" yWindow="-810" windowWidth="11850" windowHeight="9195" activeTab="2" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="135">
   <si>
     <t>Guard</t>
   </si>
@@ -372,6 +372,72 @@
   </si>
   <si>
     <t>Rockfall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cool</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Stat</t>
+  </si>
+  <si>
+    <t>Boost</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Chance</t>
+  </si>
+  <si>
+    <t>Drain</t>
+  </si>
+  <si>
+    <t>Instant Death</t>
+  </si>
+  <si>
+    <t>Reduce HP to 1</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>Vanish into Air</t>
+  </si>
+  <si>
+    <t>Double Turn</t>
+  </si>
+  <si>
+    <t>End Turn</t>
+  </si>
+  <si>
+    <t>"Lose 12% of health and may lose next turn"</t>
+  </si>
+  <si>
+    <t>May multiply damage</t>
+  </si>
+  <si>
+    <t>User Dies</t>
+  </si>
+  <si>
+    <t>Remove Condition</t>
+  </si>
+  <si>
+    <t>Param1 (string)</t>
+  </si>
+  <si>
+    <t>Param2 (int)</t>
+  </si>
+  <si>
+    <t>May ignore Defense</t>
   </si>
 </sst>
 </file>
@@ -404,12 +470,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -424,10 +508,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2B1135-77C9-499B-B6C9-9E2B30F8D34D}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,34 +854,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -894,7 +984,7 @@
         <v>26</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="M4" t="s">
         <v>26</v>
@@ -913,6 +1003,9 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
@@ -926,7 +1019,7 @@
         <v>27</v>
       </c>
       <c r="L5" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="M5" t="s">
         <v>83</v>
@@ -955,7 +1048,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B8" t="s">
@@ -967,13 +1060,13 @@
       <c r="E8" t="s">
         <v>34</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>109</v>
       </c>
       <c r="H8" t="s">
         <v>35</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="K8" t="s">
@@ -1207,7 +1300,7 @@
         <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1258,7 +1351,7 @@
         <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
@@ -1281,7 +1374,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1317,4 +1410,135 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21AE0FE-0550-4A50-A428-F4972BDBD2F3}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
quick change to offpsy to see where the error is
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet.xlsx
+++ b/IodemBot/IodemClassSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4B3976-71C0-4459-994B-6FFAAB0588FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E367D0E-6F3D-4381-B5FB-D41D2C85FB71}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5268" yWindow="1356" windowWidth="16992" windowHeight="10212" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView xWindow="5268" yWindow="1356" windowWidth="16992" windowHeight="10212" activeTab="1" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="170">
   <si>
     <t>Guard</t>
   </si>
@@ -272,9 +272,6 @@
     <t>Pharaoh</t>
   </si>
   <si>
-    <t>Desert Oracle</t>
-  </si>
-  <si>
     <t>Non-Elemental Line</t>
   </si>
   <si>
@@ -432,13 +429,127 @@
   </si>
   <si>
     <t>May ignore Defense</t>
+  </si>
+  <si>
+    <t>Dull</t>
+  </si>
+  <si>
+    <t>Pierrot</t>
+  </si>
+  <si>
+    <t>Sabre Dance</t>
+  </si>
+  <si>
+    <t>Juggle</t>
+  </si>
+  <si>
+    <t>Backstab</t>
+  </si>
+  <si>
+    <t>Tamer</t>
+  </si>
+  <si>
+    <t>Whiplash</t>
+  </si>
+  <si>
+    <t>Estre Wood</t>
+  </si>
+  <si>
+    <t>Dark Mage</t>
+  </si>
+  <si>
+    <t>Poison Flow</t>
+  </si>
+  <si>
+    <t>Elder Wood</t>
+  </si>
+  <si>
+    <t>Card Trickser</t>
+  </si>
+  <si>
+    <t>Draconier</t>
+  </si>
+  <si>
+    <t>Proxian</t>
+  </si>
+  <si>
+    <t>Bird People</t>
+  </si>
+  <si>
+    <t>Dragon Brood</t>
+  </si>
+  <si>
+    <t>Dragon Baron</t>
+  </si>
+  <si>
+    <t>Dragon Brave</t>
+  </si>
+  <si>
+    <t>Fire Dragon</t>
+  </si>
+  <si>
+    <t>Blue Dragon</t>
+  </si>
+  <si>
+    <t>Desert Gasp</t>
+  </si>
+  <si>
+    <t>Northern Flame</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Rising Dragon</t>
+  </si>
+  <si>
+    <t>Rolling Flame</t>
+  </si>
+  <si>
+    <t>Starbust/Blast</t>
+  </si>
+  <si>
+    <t>Meteor Blow</t>
+  </si>
+  <si>
+    <t>Cage</t>
+  </si>
+  <si>
+    <t>Stun Muscle</t>
+  </si>
+  <si>
+    <t>Heat Flash</t>
+  </si>
+  <si>
+    <t>Cure(?)</t>
+  </si>
+  <si>
+    <t>Break(?)</t>
+  </si>
+  <si>
+    <t>Resist(?)</t>
+  </si>
+  <si>
+    <t>Emu/Harpy/Gryphon</t>
+  </si>
+  <si>
+    <t>Undead</t>
+  </si>
+  <si>
+    <t>Card Psynergies</t>
+  </si>
+  <si>
+    <t>Desert Prophet</t>
+  </si>
+  <si>
+    <t>Arid Curate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,8 +616,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.749992370372631"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +662,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -556,12 +681,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -573,6 +699,10 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2B1135-77C9-499B-B6C9-9E2B30F8D34D}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P15" sqref="O15:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -906,7 +1036,7 @@
     <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.21875" customWidth="1"/>
     <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.77734375" bestFit="1" customWidth="1"/>
@@ -914,29 +1044,29 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="11"/>
+      <c r="J1" s="12"/>
       <c r="K1" s="4" t="s">
         <v>2</v>
       </c>
@@ -948,175 +1078,175 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="12"/>
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="7" t="s">
+      <c r="J3" s="12"/>
+      <c r="K3" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>90</v>
+      </c>
+      <c r="R3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>98</v>
+      </c>
+      <c r="R4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>91</v>
-      </c>
-      <c r="R3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="11"/>
-      <c r="K4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="Q5" t="s">
         <v>99</v>
       </c>
-      <c r="R4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>100</v>
-      </c>
       <c r="R5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="Q6" t="s">
+        <v>91</v>
+      </c>
+      <c r="R6" t="s">
         <v>92</v>
-      </c>
-      <c r="R6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="Q7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1133,7 +1263,7 @@
         <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" t="s">
         <v>35</v>
@@ -1141,7 +1271,7 @@
       <c r="I8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="11"/>
+      <c r="J8" s="12"/>
       <c r="K8" t="s">
         <v>49</v>
       </c>
@@ -1158,315 +1288,348 @@
         <v>33</v>
       </c>
       <c r="Q8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="12"/>
+      <c r="D9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="6" t="s">
+      <c r="G9" s="12"/>
+      <c r="H9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="9" t="s">
+      <c r="J9" s="12"/>
+      <c r="K9" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="N9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="12"/>
+      <c r="D10" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="14" t="s">
+      <c r="G10" s="12"/>
+      <c r="H10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="6" t="s">
+      <c r="J10" s="12"/>
+      <c r="K10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="6" t="s">
+      <c r="M10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="6" t="s">
+      <c r="N10" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="M11" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="14" t="s">
+      <c r="N11" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12" t="s">
+      <c r="F12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="12"/>
+      <c r="H12" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="12"/>
+      <c r="K12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" t="s">
+        <v>133</v>
+      </c>
+      <c r="M15" t="s">
+        <v>137</v>
+      </c>
+      <c r="N15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" t="s">
+        <v>134</v>
+      </c>
+      <c r="M16" t="s">
+        <v>138</v>
+      </c>
+      <c r="N16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" t="s">
+        <v>135</v>
+      </c>
+      <c r="N17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L18" t="s">
+        <v>136</v>
+      </c>
+      <c r="N18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="12" t="s">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="M11" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="N11" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="8" t="s">
+      <c r="I20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C13" s="11"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C14" s="11"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="8" t="s">
+      <c r="N20" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1478,40 +1641,171 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3034823A-014A-402D-994F-F4A05E7ABD19}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>75</v>
       </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>143</v>
+      </c>
       <c r="D1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+      <c r="D4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>78</v>
+      </c>
+      <c r="E6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E14" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1537,18 +1831,18 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s">
         <v>130</v>
-      </c>
-      <c r="C1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1556,93 +1850,93 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" t="s">
-        <v>116</v>
-      </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
         <v>117</v>
       </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>118</v>
-      </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
i!classinfo and Class series descriptions
</commit_message>
<xml_diff>
--- a/IodemBot/IodemClassSheet.xlsx
+++ b/IodemBot/IodemClassSheet.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\source\repos\IodemBot\IodemBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E367D0E-6F3D-4381-B5FB-D41D2C85FB71}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318E5103-9281-41C8-9546-CAD380E67BE1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5268" yWindow="1356" windowWidth="16992" windowHeight="10212" activeTab="1" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
+    <workbookView xWindow="5268" yWindow="1356" windowWidth="16992" windowHeight="10212" activeTab="3" xr2:uid="{1DC72B9C-AF88-45DA-AAFC-49E2D3101559}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="189">
   <si>
     <t>Guard</t>
   </si>
@@ -74,9 +75,6 @@
     <t>Beam</t>
   </si>
   <si>
-    <t>Weaken</t>
-  </si>
-  <si>
     <t>Aura</t>
   </si>
   <si>
@@ -543,13 +541,73 @@
   </si>
   <si>
     <t>Arid Curate</t>
+  </si>
+  <si>
+    <t>Blaze</t>
+  </si>
+  <si>
+    <t>Thermal</t>
+  </si>
+  <si>
+    <t>Venus</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>Jupiter</t>
+  </si>
+  <si>
+    <t>Mercury</t>
+  </si>
+  <si>
+    <t>Brute/Curse Mage</t>
+  </si>
+  <si>
+    <t>Air Seer/Scrapper</t>
+  </si>
+  <si>
+    <t>Jupiter (Air)</t>
+  </si>
+  <si>
+    <t>Mercury (Aqua)</t>
+  </si>
+  <si>
+    <t>Mars (Magma)</t>
+  </si>
+  <si>
+    <t>Venus (Gaia)</t>
+  </si>
+  <si>
+    <t>Squire/Miko</t>
+  </si>
+  <si>
+    <t>Guard/FlameUser/Pirate</t>
+  </si>
+  <si>
+    <t>WindSeer/Beastling</t>
+  </si>
+  <si>
+    <t>Water Seer/Mariner/Aqua Squire</t>
+  </si>
+  <si>
+    <t>non-Venus:</t>
+  </si>
+  <si>
+    <t>non-Mars</t>
+  </si>
+  <si>
+    <t>non-Jupiter</t>
+  </si>
+  <si>
+    <t>non-Mercury</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +682,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -664,7 +730,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,7 +747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -690,7 +756,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -699,10 +764,10 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1020,7 +1085,7 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P15" sqref="O15:P15"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,29 +1109,29 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="12"/>
+      <c r="J1" s="11"/>
       <c r="K1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1082,9 +1147,9 @@
         <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="12"/>
+        <v>72</v>
+      </c>
+      <c r="C2" s="11"/>
       <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
@@ -1092,34 +1157,34 @@
         <v>11</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="G2" s="11"/>
       <c r="H2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="12"/>
+        <v>19</v>
+      </c>
+      <c r="J2" s="11"/>
       <c r="K2" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="12"/>
+      <c r="B3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="11"/>
       <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
@@ -1129,504 +1194,506 @@
       <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="12"/>
+      <c r="G3" s="11"/>
       <c r="H3" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="J3" s="11"/>
       <c r="K3" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>13</v>
+      <c r="E4" s="18" t="s">
+        <v>169</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="15" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>97</v>
+      </c>
+      <c r="R4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13" t="s">
+      <c r="J5" s="11"/>
+      <c r="K5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="L5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q5" t="s">
         <v>98</v>
       </c>
-      <c r="R4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>99</v>
-      </c>
       <c r="R5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="Q6" t="s">
+        <v>90</v>
+      </c>
+      <c r="R6" t="s">
         <v>91</v>
-      </c>
-      <c r="R6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="Q7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="12"/>
-      <c r="K8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L8" t="s">
-        <v>54</v>
-      </c>
-      <c r="M8" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" t="s">
-        <v>53</v>
-      </c>
-      <c r="O8" t="s">
-        <v>33</v>
-      </c>
       <c r="Q8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="F9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="12"/>
+        <v>19</v>
+      </c>
+      <c r="G9" s="11"/>
       <c r="H9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="10" t="s">
-        <v>48</v>
-      </c>
       <c r="L9" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="M11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="12"/>
-      <c r="H10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="9" t="s">
+      <c r="N11" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="M11" s="15" t="s">
+      <c r="B12" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N11" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="O11" s="19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="G12" s="11"/>
+      <c r="H12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="9" t="s">
+      <c r="L12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="O12" s="13" t="s">
-        <v>27</v>
+      <c r="M12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C13" s="12"/>
+      <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C14" s="12"/>
+      <c r="C14" s="11"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="6" t="s">
+      <c r="E15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="H15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="L15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="12"/>
+        <v>66</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="11"/>
       <c r="D16" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+        <v>41</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
       <c r="H16" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L17" t="s">
+        <v>134</v>
+      </c>
+      <c r="N17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L17" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="L18" t="s">
         <v>135</v>
       </c>
-      <c r="N17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="8" t="s">
+      <c r="N18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="L18" t="s">
-        <v>136</v>
-      </c>
-      <c r="N18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="E19" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
+      <c r="B20" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="9" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="8" t="s">
         <v>8</v>
       </c>
       <c r="N20" t="s">
@@ -1643,7 +1710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3034823A-014A-402D-994F-F4A05E7ABD19}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1657,93 +1724,93 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" t="s">
         <v>143</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>144</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>145</v>
-      </c>
-      <c r="F1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1751,61 +1818,61 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E12" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E13" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E14" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E15" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1831,18 +1898,18 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
         <v>129</v>
-      </c>
-      <c r="C1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1850,97 +1917,237 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
         <v>114</v>
       </c>
-      <c r="B4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>115</v>
-      </c>
       <c r="E4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
         <v>116</v>
       </c>
-      <c r="B5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" t="s">
-        <v>117</v>
-      </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B53968-0167-4F4F-BD4B-0794225E238B}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>